<commit_message>
mybatis dynamic sql 测试
</commit_message>
<xml_diff>
--- a/src/main/demo/学生信息表.xlsx
+++ b/src/main/demo/学生信息表.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="21">
   <si>
     <t>学号</t>
   </si>
@@ -48,6 +48,48 @@
   </si>
   <si>
     <t>女</t>
+  </si>
+  <si>
+    <t>0010002</t>
+  </si>
+  <si>
+    <t>张四</t>
+  </si>
+  <si>
+    <t>0010003</t>
+  </si>
+  <si>
+    <t>流量</t>
+  </si>
+  <si>
+    <t>0010004</t>
+  </si>
+  <si>
+    <t>驴</t>
+  </si>
+  <si>
+    <t>0010005</t>
+  </si>
+  <si>
+    <t>驴2</t>
+  </si>
+  <si>
+    <t>0010006</t>
+  </si>
+  <si>
+    <t>李老师</t>
+  </si>
+  <si>
+    <t>0010007</t>
+  </si>
+  <si>
+    <t>达到</t>
+  </si>
+  <si>
+    <t>0010008</t>
+  </si>
+  <si>
+    <t>张三2</t>
   </si>
 </sst>
 </file>
@@ -60,14 +102,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -523,148 +558,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -991,13 +1026,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D8" sqref="D8:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelCol="3"/>
   <cols>
     <col min="4" max="4" width="9.22222222222222"/>
   </cols>
@@ -1030,6 +1065,104 @@
         <v>40910</v>
       </c>
     </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1">
+        <v>40911</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1">
+        <v>40912</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1">
+        <v>40913</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="1">
+        <v>40914</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1">
+        <v>40915</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="1">
+        <v>40916</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="1">
+        <v>40917</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>